<commit_message>
added cpl file (positions.csv), updated BOM excel sheet, turned gerbers into zip file
</commit_message>
<xml_diff>
--- a/BOM for JLCPCB Assembly.xlsx
+++ b/BOM for JLCPCB Assembly.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6ac1be91de688dc1/Desktop/leaderboard/Controls-LeaderPCB/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucyx\OneDrive\Documents\GitHub\Controls-LeaderPCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_F25DC773A252ABDACC1048DA491B4E2C5ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62860840-6FB9-4BEE-A754-1122D44B1215}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F000D4C3-CD48-4E24-A73C-C34D534CEB1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="157">
   <si>
     <t xml:space="preserve">Comment </t>
   </si>
@@ -45,9 +45,6 @@
     <t>1u</t>
   </si>
   <si>
-    <t>C1-C4, C15, C32</t>
-  </si>
-  <si>
     <t>Capacitor_SMD:C_0805_2012Metric</t>
   </si>
   <si>
@@ -57,63 +54,42 @@
     <t>100nF</t>
   </si>
   <si>
-    <t>C5, C6, C9, C11, C12, C14, C16-C19, C24, C25, C29, C34, C35, C39, C42</t>
-  </si>
-  <si>
     <t>C49678</t>
   </si>
   <si>
     <t>12pF</t>
   </si>
   <si>
-    <t>C7, C8</t>
-  </si>
-  <si>
     <t>C376863</t>
   </si>
   <si>
     <t>4.7uF</t>
   </si>
   <si>
-    <t>C10, C13, C41</t>
-  </si>
-  <si>
     <t>C1779</t>
   </si>
   <si>
     <t>10u</t>
   </si>
   <si>
-    <t>C20-C23, C28, C33, C38</t>
-  </si>
-  <si>
     <t>C15850</t>
   </si>
   <si>
     <t>0.01uF</t>
   </si>
   <si>
-    <t>C26, C30, C36, C40</t>
-  </si>
-  <si>
     <t>C1710</t>
   </si>
   <si>
     <t>0.22uF</t>
   </si>
   <si>
-    <t>C27, C37</t>
-  </si>
-  <si>
     <t>C5378</t>
   </si>
   <si>
     <t>BAS70-04</t>
   </si>
   <si>
-    <t>D2-D5</t>
-  </si>
-  <si>
     <t>Package_TO_SOT_SMD:SOT-23</t>
   </si>
   <si>
@@ -135,9 +111,6 @@
     <t>PowerOn</t>
   </si>
   <si>
-    <t>D8, D14</t>
-  </si>
-  <si>
     <t>LED_SMD:LED_0805_2012Metric</t>
   </si>
   <si>
@@ -156,48 +129,24 @@
     <t>C3040626</t>
   </si>
   <si>
-    <t>2kH</t>
-  </si>
-  <si>
-    <t>L5-L8</t>
-  </si>
-  <si>
-    <t>Inductor_SMD:L_0805_2012Metric</t>
-  </si>
-  <si>
-    <t>NOT ON JLC (mouser #: 623-2508051527Y0)</t>
-  </si>
-  <si>
-    <t>R1-R4, R24-R27</t>
-  </si>
-  <si>
     <t>Resistor_SMD:R_0805_2012Metric</t>
   </si>
   <si>
     <t>C2933517</t>
   </si>
   <si>
-    <t>R5, R6</t>
-  </si>
-  <si>
     <t>C17408</t>
   </si>
   <si>
     <t>1.5k</t>
   </si>
   <si>
-    <t>R7, R29</t>
-  </si>
-  <si>
     <t>C4310</t>
   </si>
   <si>
     <t>5k</t>
   </si>
   <si>
-    <t>R10, R11</t>
-  </si>
-  <si>
     <t>1.2k</t>
   </si>
   <si>
@@ -210,30 +159,18 @@
     <t>5.1k</t>
   </si>
   <si>
-    <t>R13, R14, R19, R20</t>
-  </si>
-  <si>
     <t>C27834</t>
   </si>
   <si>
     <t>10k</t>
   </si>
   <si>
-    <t>R15, R16, R18, R22, R23</t>
-  </si>
-  <si>
     <t>C17414</t>
   </si>
   <si>
-    <t>R17, R34</t>
-  </si>
-  <si>
     <t>C17477</t>
   </si>
   <si>
-    <t>R21, R35</t>
-  </si>
-  <si>
     <t>C17437</t>
   </si>
   <si>
@@ -276,18 +213,6 @@
     <t>C2690020</t>
   </si>
   <si>
-    <t>STM32F413RHTx</t>
-  </si>
-  <si>
-    <t>U7</t>
-  </si>
-  <si>
-    <t>Package_QFP:LQFP-64_10x10mm_P0.5mm</t>
-  </si>
-  <si>
-    <t>C2969899</t>
-  </si>
-  <si>
     <t>NCP1117-3.3_SOT223</t>
   </si>
   <si>
@@ -303,9 +228,6 @@
     <t>ADM3055E</t>
   </si>
   <si>
-    <t>U14, U17</t>
-  </si>
-  <si>
     <t>UTSVT_ICs:SOIC-20W_7.5x15.4mm_Pitch1.27mm</t>
   </si>
   <si>
@@ -315,9 +237,6 @@
     <t>CDSOT23-T24CAN</t>
   </si>
   <si>
-    <t>U15, U18</t>
-  </si>
-  <si>
     <t>Package_TO_SOT_SMD:SOT-23W</t>
   </si>
   <si>
@@ -346,13 +265,244 @@
   </si>
   <si>
     <t>C144380</t>
+  </si>
+  <si>
+    <t>C2828700</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C32</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>C16</t>
+  </si>
+  <si>
+    <t>C17</t>
+  </si>
+  <si>
+    <t>C18</t>
+  </si>
+  <si>
+    <t>C19</t>
+  </si>
+  <si>
+    <t>C24</t>
+  </si>
+  <si>
+    <t>C25</t>
+  </si>
+  <si>
+    <t>C29</t>
+  </si>
+  <si>
+    <t>C34</t>
+  </si>
+  <si>
+    <t>C35</t>
+  </si>
+  <si>
+    <t>C39</t>
+  </si>
+  <si>
+    <t>C42</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>C13</t>
+  </si>
+  <si>
+    <t>C41</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>C21</t>
+  </si>
+  <si>
+    <t>C22</t>
+  </si>
+  <si>
+    <t>C23</t>
+  </si>
+  <si>
+    <t>C28</t>
+  </si>
+  <si>
+    <t>C33</t>
+  </si>
+  <si>
+    <t>C38</t>
+  </si>
+  <si>
+    <t>C20</t>
+  </si>
+  <si>
+    <t>C30</t>
+  </si>
+  <si>
+    <t>C36</t>
+  </si>
+  <si>
+    <t>C40</t>
+  </si>
+  <si>
+    <t>C26</t>
+  </si>
+  <si>
+    <t>C37</t>
+  </si>
+  <si>
+    <t>C27</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>D5</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>D14</t>
+  </si>
+  <si>
+    <t>D8</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>R24</t>
+  </si>
+  <si>
+    <t>R25</t>
+  </si>
+  <si>
+    <t>R26</t>
+  </si>
+  <si>
+    <t>R27</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>R29</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>R19</t>
+  </si>
+  <si>
+    <t>R20</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>R16</t>
+  </si>
+  <si>
+    <t>R18</t>
+  </si>
+  <si>
+    <t>R22</t>
+  </si>
+  <si>
+    <t>R23</t>
+  </si>
+  <si>
+    <t>R15</t>
+  </si>
+  <si>
+    <t>R34</t>
+  </si>
+  <si>
+    <t>R17</t>
+  </si>
+  <si>
+    <t>R35</t>
+  </si>
+  <si>
+    <t>R21</t>
+  </si>
+  <si>
+    <t>U17</t>
+  </si>
+  <si>
+    <t>U14</t>
+  </si>
+  <si>
+    <t>U18</t>
+  </si>
+  <si>
+    <t>U15</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -375,12 +525,6 @@
       <sz val="10"/>
       <color rgb="FF222222"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -452,7 +596,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -488,15 +632,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -787,13 +922,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S32"/>
+  <dimension ref="A1:S87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U11" sqref="U11"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="18" max="18" width="0" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="8.88671875" hidden="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -833,13 +972,13 @@
       <c r="B2" s="10"/>
       <c r="C2" s="11"/>
       <c r="D2" s="9" t="s">
-        <v>6</v>
+        <v>85</v>
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
       <c r="G2" s="11"/>
       <c r="H2" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I2" s="13"/>
       <c r="J2" s="13"/>
@@ -848,7 +987,7 @@
       <c r="M2" s="13"/>
       <c r="N2" s="14"/>
       <c r="O2" s="12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="P2" s="13"/>
       <c r="Q2" s="14"/>
@@ -859,18 +998,18 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="11"/>
       <c r="D3" s="9" t="s">
-        <v>10</v>
+        <v>81</v>
       </c>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
       <c r="G3" s="11"/>
       <c r="H3" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I3" s="13"/>
       <c r="J3" s="13"/>
@@ -878,30 +1017,30 @@
       <c r="L3" s="13"/>
       <c r="M3" s="13"/>
       <c r="N3" s="14"/>
-      <c r="O3" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="P3" s="16"/>
-      <c r="Q3" s="17"/>
+      <c r="O3" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="14"/>
       <c r="R3" s="12">
-        <v>6507420</v>
+        <v>647623</v>
       </c>
       <c r="S3" s="14"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="11"/>
       <c r="D4" s="9" t="s">
-        <v>13</v>
+        <v>82</v>
       </c>
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
       <c r="G4" s="11"/>
       <c r="H4" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I4" s="13"/>
       <c r="J4" s="13"/>
@@ -910,29 +1049,29 @@
       <c r="M4" s="13"/>
       <c r="N4" s="14"/>
       <c r="O4" s="12" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="P4" s="13"/>
       <c r="Q4" s="14"/>
       <c r="R4" s="12">
-        <v>3913</v>
+        <v>647623</v>
       </c>
       <c r="S4" s="14"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="11"/>
       <c r="D5" s="9" t="s">
-        <v>16</v>
+        <v>83</v>
       </c>
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
       <c r="G5" s="11"/>
       <c r="H5" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I5" s="13"/>
       <c r="J5" s="13"/>
@@ -941,29 +1080,29 @@
       <c r="M5" s="13"/>
       <c r="N5" s="14"/>
       <c r="O5" s="12" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="P5" s="13"/>
       <c r="Q5" s="14"/>
       <c r="R5" s="12">
-        <v>2094551</v>
+        <v>647623</v>
       </c>
       <c r="S5" s="14"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="11"/>
       <c r="D6" s="9" t="s">
-        <v>19</v>
+        <v>84</v>
       </c>
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
       <c r="G6" s="11"/>
       <c r="H6" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I6" s="13"/>
       <c r="J6" s="13"/>
@@ -972,29 +1111,29 @@
       <c r="M6" s="13"/>
       <c r="N6" s="14"/>
       <c r="O6" s="12" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="P6" s="13"/>
       <c r="Q6" s="14"/>
       <c r="R6" s="12">
-        <v>5148770</v>
+        <v>647623</v>
       </c>
       <c r="S6" s="14"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="11"/>
       <c r="D7" s="9" t="s">
-        <v>22</v>
+        <v>101</v>
       </c>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
       <c r="G7" s="11"/>
       <c r="H7" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I7" s="13"/>
       <c r="J7" s="13"/>
@@ -1002,30 +1141,30 @@
       <c r="L7" s="13"/>
       <c r="M7" s="13"/>
       <c r="N7" s="14"/>
-      <c r="O7" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="14"/>
+      <c r="O7" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="17"/>
       <c r="R7" s="12">
-        <v>518880</v>
+        <v>6507420</v>
       </c>
       <c r="S7" s="14"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="11"/>
       <c r="D8" s="9" t="s">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
       <c r="G8" s="11"/>
       <c r="H8" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I8" s="13"/>
       <c r="J8" s="13"/>
@@ -1033,30 +1172,30 @@
       <c r="L8" s="13"/>
       <c r="M8" s="13"/>
       <c r="N8" s="14"/>
-      <c r="O8" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="P8" s="13"/>
-      <c r="Q8" s="14"/>
+      <c r="O8" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="17"/>
       <c r="R8" s="12">
-        <v>135203</v>
+        <v>6507420</v>
       </c>
       <c r="S8" s="14"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="D9" s="9" t="s">
-        <v>28</v>
+        <v>87</v>
       </c>
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
       <c r="G9" s="11"/>
       <c r="H9" s="12" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="I9" s="13"/>
       <c r="J9" s="13"/>
@@ -1064,30 +1203,30 @@
       <c r="L9" s="13"/>
       <c r="M9" s="13"/>
       <c r="N9" s="14"/>
-      <c r="O9" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="P9" s="13"/>
-      <c r="Q9" s="14"/>
+      <c r="O9" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="17"/>
       <c r="R9" s="12">
-        <v>24530</v>
+        <v>6507420</v>
       </c>
       <c r="S9" s="14"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="D10" s="9" t="s">
-        <v>32</v>
+        <v>88</v>
       </c>
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
       <c r="G10" s="11"/>
       <c r="H10" s="12" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="I10" s="13"/>
       <c r="J10" s="13"/>
@@ -1095,30 +1234,30 @@
       <c r="L10" s="13"/>
       <c r="M10" s="13"/>
       <c r="N10" s="14"/>
-      <c r="O10" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="P10" s="13"/>
-      <c r="Q10" s="14"/>
+      <c r="O10" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="17"/>
       <c r="R10" s="12">
-        <v>833</v>
+        <v>6507420</v>
       </c>
       <c r="S10" s="14"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="D11" s="9" t="s">
-        <v>36</v>
+        <v>89</v>
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
       <c r="G11" s="11"/>
       <c r="H11" s="12" t="s">
-        <v>37</v>
+        <v>6</v>
       </c>
       <c r="I11" s="13"/>
       <c r="J11" s="13"/>
@@ -1126,30 +1265,30 @@
       <c r="L11" s="13"/>
       <c r="M11" s="13"/>
       <c r="N11" s="14"/>
-      <c r="O11" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="P11" s="13"/>
-      <c r="Q11" s="14"/>
+      <c r="O11" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="P11" s="16"/>
+      <c r="Q11" s="17"/>
       <c r="R11" s="12">
-        <v>3139</v>
+        <v>6507420</v>
       </c>
       <c r="S11" s="14"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="D12" s="9" t="s">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
       <c r="G12" s="11"/>
       <c r="H12" s="12" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="I12" s="13"/>
       <c r="J12" s="13"/>
@@ -1157,30 +1296,30 @@
       <c r="L12" s="13"/>
       <c r="M12" s="13"/>
       <c r="N12" s="14"/>
-      <c r="O12" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="P12" s="13"/>
-      <c r="Q12" s="14"/>
+      <c r="O12" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="17"/>
       <c r="R12" s="12">
-        <v>120289</v>
+        <v>6507420</v>
       </c>
       <c r="S12" s="14"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="D13" s="9" t="s">
-        <v>44</v>
+        <v>91</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
       <c r="G13" s="11"/>
       <c r="H13" s="12" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="I13" s="13"/>
       <c r="J13" s="13"/>
@@ -1188,28 +1327,30 @@
       <c r="L13" s="13"/>
       <c r="M13" s="13"/>
       <c r="N13" s="14"/>
-      <c r="O13" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="P13" s="13"/>
-      <c r="Q13" s="14"/>
-      <c r="R13" s="12"/>
+      <c r="O13" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="P13" s="16"/>
+      <c r="Q13" s="17"/>
+      <c r="R13" s="12">
+        <v>6507420</v>
+      </c>
       <c r="S13" s="14"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A14" s="9">
-        <v>110</v>
+      <c r="A14" s="9" t="s">
+        <v>8</v>
       </c>
       <c r="B14" s="10"/>
       <c r="C14" s="11"/>
       <c r="D14" s="9" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
       <c r="G14" s="11"/>
       <c r="H14" s="12" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="I14" s="13"/>
       <c r="J14" s="13"/>
@@ -1217,30 +1358,30 @@
       <c r="L14" s="13"/>
       <c r="M14" s="13"/>
       <c r="N14" s="14"/>
-      <c r="O14" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="P14" s="13"/>
-      <c r="Q14" s="14"/>
+      <c r="O14" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="P14" s="16"/>
+      <c r="Q14" s="17"/>
       <c r="R14" s="12">
-        <v>844</v>
+        <v>6507420</v>
       </c>
       <c r="S14" s="14"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A15" s="9">
-        <v>510</v>
+      <c r="A15" s="9" t="s">
+        <v>8</v>
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="11"/>
       <c r="D15" s="9" t="s">
-        <v>50</v>
+        <v>93</v>
       </c>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
       <c r="G15" s="11"/>
       <c r="H15" s="12" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="I15" s="13"/>
       <c r="J15" s="13"/>
@@ -1248,30 +1389,30 @@
       <c r="L15" s="13"/>
       <c r="M15" s="13"/>
       <c r="N15" s="14"/>
-      <c r="O15" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="P15" s="13"/>
-      <c r="Q15" s="14"/>
+      <c r="O15" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="P15" s="16"/>
+      <c r="Q15" s="17"/>
       <c r="R15" s="12">
-        <v>1400280</v>
+        <v>6507420</v>
       </c>
       <c r="S15" s="14"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="11"/>
       <c r="D16" s="9" t="s">
-        <v>53</v>
+        <v>94</v>
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="11"/>
       <c r="H16" s="12" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="I16" s="13"/>
       <c r="J16" s="13"/>
@@ -1279,30 +1420,30 @@
       <c r="L16" s="13"/>
       <c r="M16" s="13"/>
       <c r="N16" s="14"/>
-      <c r="O16" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="P16" s="13"/>
-      <c r="Q16" s="14"/>
+      <c r="O16" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="17"/>
       <c r="R16" s="12">
-        <v>436191</v>
+        <v>6507420</v>
       </c>
       <c r="S16" s="14"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="B17" s="10"/>
       <c r="C17" s="11"/>
       <c r="D17" s="9" t="s">
-        <v>56</v>
+        <v>95</v>
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="11"/>
       <c r="H17" s="12" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="I17" s="13"/>
       <c r="J17" s="13"/>
@@ -1310,11 +1451,11 @@
       <c r="L17" s="13"/>
       <c r="M17" s="13"/>
       <c r="N17" s="14"/>
-      <c r="O17" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="P17" s="13"/>
-      <c r="Q17" s="14"/>
+      <c r="O17" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="P17" s="16"/>
+      <c r="Q17" s="17"/>
       <c r="R17" s="12">
         <v>6507420</v>
       </c>
@@ -1322,18 +1463,18 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="B18" s="10"/>
       <c r="C18" s="11"/>
       <c r="D18" s="9" t="s">
-        <v>58</v>
+        <v>96</v>
       </c>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="11"/>
       <c r="H18" s="12" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="I18" s="13"/>
       <c r="J18" s="13"/>
@@ -1341,30 +1482,30 @@
       <c r="L18" s="13"/>
       <c r="M18" s="13"/>
       <c r="N18" s="14"/>
-      <c r="O18" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="P18" s="13"/>
-      <c r="Q18" s="14"/>
+      <c r="O18" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="P18" s="16"/>
+      <c r="Q18" s="17"/>
       <c r="R18" s="12">
-        <v>163751</v>
+        <v>6507420</v>
       </c>
       <c r="S18" s="14"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>60</v>
+        <v>8</v>
       </c>
       <c r="B19" s="10"/>
       <c r="C19" s="11"/>
       <c r="D19" s="9" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
       <c r="G19" s="11"/>
       <c r="H19" s="12" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="I19" s="13"/>
       <c r="J19" s="13"/>
@@ -1372,30 +1513,30 @@
       <c r="L19" s="13"/>
       <c r="M19" s="13"/>
       <c r="N19" s="14"/>
-      <c r="O19" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="P19" s="13"/>
-      <c r="Q19" s="14"/>
+      <c r="O19" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="P19" s="16"/>
+      <c r="Q19" s="17"/>
       <c r="R19" s="12">
-        <v>693108</v>
+        <v>6507420</v>
       </c>
       <c r="S19" s="14"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="B20" s="10"/>
       <c r="C20" s="11"/>
       <c r="D20" s="9" t="s">
-        <v>64</v>
+        <v>98</v>
       </c>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
       <c r="G20" s="11"/>
       <c r="H20" s="12" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="I20" s="13"/>
       <c r="J20" s="13"/>
@@ -1403,30 +1544,30 @@
       <c r="L20" s="13"/>
       <c r="M20" s="13"/>
       <c r="N20" s="14"/>
-      <c r="O20" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="P20" s="13"/>
-      <c r="Q20" s="14"/>
+      <c r="O20" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="P20" s="16"/>
+      <c r="Q20" s="17"/>
       <c r="R20" s="12">
-        <v>18834045</v>
+        <v>6507420</v>
       </c>
       <c r="S20" s="14"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A21" s="9">
-        <v>0</v>
+      <c r="A21" s="9" t="s">
+        <v>8</v>
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="11"/>
       <c r="D21" s="9" t="s">
-        <v>66</v>
+        <v>99</v>
       </c>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
       <c r="G21" s="11"/>
       <c r="H21" s="12" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="I21" s="13"/>
       <c r="J21" s="13"/>
@@ -1434,30 +1575,30 @@
       <c r="L21" s="13"/>
       <c r="M21" s="13"/>
       <c r="N21" s="14"/>
-      <c r="O21" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="P21" s="13"/>
-      <c r="Q21" s="14"/>
+      <c r="O21" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="P21" s="16"/>
+      <c r="Q21" s="17"/>
       <c r="R21" s="12">
-        <v>1157685</v>
+        <v>6507420</v>
       </c>
       <c r="S21" s="14"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A22" s="9">
-        <v>120</v>
+      <c r="A22" s="9" t="s">
+        <v>8</v>
       </c>
       <c r="B22" s="10"/>
       <c r="C22" s="11"/>
       <c r="D22" s="9" t="s">
-        <v>68</v>
+        <v>100</v>
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
       <c r="G22" s="11"/>
       <c r="H22" s="12" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="I22" s="13"/>
       <c r="J22" s="13"/>
@@ -1465,30 +1606,30 @@
       <c r="L22" s="13"/>
       <c r="M22" s="13"/>
       <c r="N22" s="14"/>
-      <c r="O22" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="P22" s="13"/>
-      <c r="Q22" s="14"/>
+      <c r="O22" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="P22" s="16"/>
+      <c r="Q22" s="17"/>
       <c r="R22" s="12">
-        <v>303844</v>
+        <v>6507420</v>
       </c>
       <c r="S22" s="14"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="B23" s="10"/>
       <c r="C23" s="11"/>
       <c r="D23" s="9" t="s">
-        <v>71</v>
+        <v>103</v>
       </c>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
       <c r="G23" s="11"/>
       <c r="H23" s="12" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="I23" s="13"/>
       <c r="J23" s="13"/>
@@ -1497,29 +1638,29 @@
       <c r="M23" s="13"/>
       <c r="N23" s="14"/>
       <c r="O23" s="12" t="s">
-        <v>72</v>
+        <v>11</v>
       </c>
       <c r="P23" s="13"/>
       <c r="Q23" s="14"/>
       <c r="R23" s="12">
-        <v>50</v>
+        <v>3913</v>
       </c>
       <c r="S23" s="14"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
-        <v>73</v>
+        <v>10</v>
       </c>
       <c r="B24" s="10"/>
       <c r="C24" s="11"/>
       <c r="D24" s="9" t="s">
-        <v>74</v>
+        <v>102</v>
       </c>
       <c r="E24" s="10"/>
       <c r="F24" s="10"/>
       <c r="G24" s="11"/>
       <c r="H24" s="12" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="I24" s="13"/>
       <c r="J24" s="13"/>
@@ -1528,29 +1669,29 @@
       <c r="M24" s="13"/>
       <c r="N24" s="14"/>
       <c r="O24" s="12" t="s">
-        <v>75</v>
+        <v>11</v>
       </c>
       <c r="P24" s="13"/>
       <c r="Q24" s="14"/>
       <c r="R24" s="12">
-        <v>2177</v>
+        <v>3913</v>
       </c>
       <c r="S24" s="14"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
-        <v>76</v>
+        <v>12</v>
       </c>
       <c r="B25" s="10"/>
       <c r="C25" s="11"/>
       <c r="D25" s="9" t="s">
-        <v>77</v>
+        <v>106</v>
       </c>
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
       <c r="G25" s="11"/>
       <c r="H25" s="12" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="I25" s="13"/>
       <c r="J25" s="13"/>
@@ -1559,29 +1700,29 @@
       <c r="M25" s="13"/>
       <c r="N25" s="14"/>
       <c r="O25" s="12" t="s">
-        <v>78</v>
+        <v>13</v>
       </c>
       <c r="P25" s="13"/>
       <c r="Q25" s="14"/>
       <c r="R25" s="12">
-        <v>9841243</v>
+        <v>2094551</v>
       </c>
       <c r="S25" s="14"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
-        <v>79</v>
+        <v>12</v>
       </c>
       <c r="B26" s="10"/>
       <c r="C26" s="11"/>
       <c r="D26" s="9" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
       <c r="G26" s="11"/>
       <c r="H26" s="12" t="s">
-        <v>81</v>
+        <v>6</v>
       </c>
       <c r="I26" s="13"/>
       <c r="J26" s="13"/>
@@ -1590,29 +1731,29 @@
       <c r="M26" s="13"/>
       <c r="N26" s="14"/>
       <c r="O26" s="12" t="s">
-        <v>82</v>
+        <v>13</v>
       </c>
       <c r="P26" s="13"/>
       <c r="Q26" s="14"/>
       <c r="R26" s="12">
-        <v>1753</v>
+        <v>2094551</v>
       </c>
       <c r="S26" s="14"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
-        <v>83</v>
+        <v>12</v>
       </c>
       <c r="B27" s="10"/>
       <c r="C27" s="11"/>
       <c r="D27" s="9" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
       <c r="G27" s="11"/>
       <c r="H27" s="12" t="s">
-        <v>85</v>
+        <v>6</v>
       </c>
       <c r="I27" s="13"/>
       <c r="J27" s="13"/>
@@ -1620,30 +1761,30 @@
       <c r="L27" s="13"/>
       <c r="M27" s="13"/>
       <c r="N27" s="14"/>
-      <c r="O27" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="P27" s="19"/>
-      <c r="Q27" s="20"/>
-      <c r="R27" s="21">
-        <v>1</v>
-      </c>
-      <c r="S27" s="22"/>
+      <c r="O27" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="P27" s="13"/>
+      <c r="Q27" s="14"/>
+      <c r="R27" s="12">
+        <v>2094551</v>
+      </c>
+      <c r="S27" s="14"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
-        <v>87</v>
+        <v>14</v>
       </c>
       <c r="B28" s="10"/>
       <c r="C28" s="11"/>
       <c r="D28" s="9" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
       <c r="G28" s="11"/>
       <c r="H28" s="12" t="s">
-        <v>89</v>
+        <v>6</v>
       </c>
       <c r="I28" s="13"/>
       <c r="J28" s="13"/>
@@ -1652,29 +1793,29 @@
       <c r="M28" s="13"/>
       <c r="N28" s="14"/>
       <c r="O28" s="12" t="s">
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="P28" s="13"/>
       <c r="Q28" s="14"/>
       <c r="R28" s="12">
-        <v>3625</v>
+        <v>5148770</v>
       </c>
       <c r="S28" s="14"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
-        <v>91</v>
+        <v>14</v>
       </c>
       <c r="B29" s="10"/>
       <c r="C29" s="11"/>
       <c r="D29" s="9" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
       <c r="G29" s="11"/>
       <c r="H29" s="12" t="s">
-        <v>93</v>
+        <v>6</v>
       </c>
       <c r="I29" s="13"/>
       <c r="J29" s="13"/>
@@ -1683,29 +1824,29 @@
       <c r="M29" s="13"/>
       <c r="N29" s="14"/>
       <c r="O29" s="12" t="s">
-        <v>94</v>
+        <v>15</v>
       </c>
       <c r="P29" s="13"/>
       <c r="Q29" s="14"/>
       <c r="R29" s="12">
-        <v>314</v>
+        <v>5148770</v>
       </c>
       <c r="S29" s="14"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
-        <v>95</v>
+        <v>14</v>
       </c>
       <c r="B30" s="10"/>
       <c r="C30" s="11"/>
       <c r="D30" s="9" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="E30" s="10"/>
       <c r="F30" s="10"/>
       <c r="G30" s="11"/>
       <c r="H30" s="12" t="s">
-        <v>97</v>
+        <v>6</v>
       </c>
       <c r="I30" s="13"/>
       <c r="J30" s="13"/>
@@ -1714,29 +1855,29 @@
       <c r="M30" s="13"/>
       <c r="N30" s="14"/>
       <c r="O30" s="12" t="s">
-        <v>98</v>
+        <v>15</v>
       </c>
       <c r="P30" s="13"/>
       <c r="Q30" s="14"/>
       <c r="R30" s="12">
-        <v>5671</v>
+        <v>5148770</v>
       </c>
       <c r="S30" s="14"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A31" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="B31" s="24"/>
-      <c r="C31" s="25"/>
+      <c r="A31" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" s="10"/>
+      <c r="C31" s="11"/>
       <c r="D31" s="9" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
       <c r="G31" s="11"/>
       <c r="H31" s="12" t="s">
-        <v>101</v>
+        <v>6</v>
       </c>
       <c r="I31" s="13"/>
       <c r="J31" s="13"/>
@@ -1745,29 +1886,29 @@
       <c r="M31" s="13"/>
       <c r="N31" s="14"/>
       <c r="O31" s="12" t="s">
-        <v>102</v>
+        <v>15</v>
       </c>
       <c r="P31" s="13"/>
       <c r="Q31" s="14"/>
       <c r="R31" s="12">
-        <v>4172</v>
+        <v>5148770</v>
       </c>
       <c r="S31" s="14"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
-        <v>103</v>
+        <v>14</v>
       </c>
       <c r="B32" s="10"/>
       <c r="C32" s="11"/>
       <c r="D32" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="E32" s="10"/>
       <c r="F32" s="10"/>
       <c r="G32" s="11"/>
       <c r="H32" s="12" t="s">
-        <v>105</v>
+        <v>6</v>
       </c>
       <c r="I32" s="13"/>
       <c r="J32" s="13"/>
@@ -1776,67 +1917,1879 @@
       <c r="M32" s="13"/>
       <c r="N32" s="14"/>
       <c r="O32" s="12" t="s">
-        <v>106</v>
+        <v>15</v>
       </c>
       <c r="P32" s="13"/>
       <c r="Q32" s="14"/>
       <c r="R32" s="12">
+        <v>5148770</v>
+      </c>
+      <c r="S32" s="14"/>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A33" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" s="10"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I33" s="13"/>
+      <c r="J33" s="13"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="13"/>
+      <c r="M33" s="13"/>
+      <c r="N33" s="14"/>
+      <c r="O33" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="P33" s="13"/>
+      <c r="Q33" s="14"/>
+      <c r="R33" s="12">
+        <v>5148770</v>
+      </c>
+      <c r="S33" s="14"/>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A34" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" s="10"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13"/>
+      <c r="M34" s="13"/>
+      <c r="N34" s="14"/>
+      <c r="O34" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="P34" s="13"/>
+      <c r="Q34" s="14"/>
+      <c r="R34" s="12">
+        <v>5148770</v>
+      </c>
+      <c r="S34" s="14"/>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A35" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" s="10"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I35" s="13"/>
+      <c r="J35" s="13"/>
+      <c r="K35" s="13"/>
+      <c r="L35" s="13"/>
+      <c r="M35" s="13"/>
+      <c r="N35" s="14"/>
+      <c r="O35" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="P35" s="13"/>
+      <c r="Q35" s="14"/>
+      <c r="R35" s="12">
+        <v>518880</v>
+      </c>
+      <c r="S35" s="14"/>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A36" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" s="10"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I36" s="13"/>
+      <c r="J36" s="13"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
+      <c r="M36" s="13"/>
+      <c r="N36" s="14"/>
+      <c r="O36" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="P36" s="13"/>
+      <c r="Q36" s="14"/>
+      <c r="R36" s="12">
+        <v>518880</v>
+      </c>
+      <c r="S36" s="14"/>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A37" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37" s="10"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13"/>
+      <c r="K37" s="13"/>
+      <c r="L37" s="13"/>
+      <c r="M37" s="13"/>
+      <c r="N37" s="14"/>
+      <c r="O37" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="P37" s="13"/>
+      <c r="Q37" s="14"/>
+      <c r="R37" s="12">
+        <v>518880</v>
+      </c>
+      <c r="S37" s="14"/>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A38" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38" s="10"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I38" s="13"/>
+      <c r="J38" s="13"/>
+      <c r="K38" s="13"/>
+      <c r="L38" s="13"/>
+      <c r="M38" s="13"/>
+      <c r="N38" s="14"/>
+      <c r="O38" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="P38" s="13"/>
+      <c r="Q38" s="14"/>
+      <c r="R38" s="12">
+        <v>518880</v>
+      </c>
+      <c r="S38" s="14"/>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A39" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B39" s="10"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I39" s="13"/>
+      <c r="J39" s="13"/>
+      <c r="K39" s="13"/>
+      <c r="L39" s="13"/>
+      <c r="M39" s="13"/>
+      <c r="N39" s="14"/>
+      <c r="O39" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="P39" s="13"/>
+      <c r="Q39" s="14"/>
+      <c r="R39" s="12">
+        <v>135203</v>
+      </c>
+      <c r="S39" s="14"/>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A40" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B40" s="10"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I40" s="13"/>
+      <c r="J40" s="13"/>
+      <c r="K40" s="13"/>
+      <c r="L40" s="13"/>
+      <c r="M40" s="13"/>
+      <c r="N40" s="14"/>
+      <c r="O40" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="P40" s="13"/>
+      <c r="Q40" s="14"/>
+      <c r="R40" s="12">
+        <v>135203</v>
+      </c>
+      <c r="S40" s="14"/>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A41" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B41" s="10"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I41" s="13"/>
+      <c r="J41" s="13"/>
+      <c r="K41" s="13"/>
+      <c r="L41" s="13"/>
+      <c r="M41" s="13"/>
+      <c r="N41" s="14"/>
+      <c r="O41" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="P41" s="13"/>
+      <c r="Q41" s="14"/>
+      <c r="R41" s="12">
+        <v>24530</v>
+      </c>
+      <c r="S41" s="14"/>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A42" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B42" s="10"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I42" s="13"/>
+      <c r="J42" s="13"/>
+      <c r="K42" s="13"/>
+      <c r="L42" s="13"/>
+      <c r="M42" s="13"/>
+      <c r="N42" s="14"/>
+      <c r="O42" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="P42" s="13"/>
+      <c r="Q42" s="14"/>
+      <c r="R42" s="12">
+        <v>24530</v>
+      </c>
+      <c r="S42" s="14"/>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A43" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B43" s="10"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I43" s="13"/>
+      <c r="J43" s="13"/>
+      <c r="K43" s="13"/>
+      <c r="L43" s="13"/>
+      <c r="M43" s="13"/>
+      <c r="N43" s="14"/>
+      <c r="O43" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="P43" s="13"/>
+      <c r="Q43" s="14"/>
+      <c r="R43" s="12">
+        <v>24530</v>
+      </c>
+      <c r="S43" s="14"/>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A44" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B44" s="10"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="E44" s="10"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I44" s="13"/>
+      <c r="J44" s="13"/>
+      <c r="K44" s="13"/>
+      <c r="L44" s="13"/>
+      <c r="M44" s="13"/>
+      <c r="N44" s="14"/>
+      <c r="O44" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="P44" s="13"/>
+      <c r="Q44" s="14"/>
+      <c r="R44" s="12">
+        <v>24530</v>
+      </c>
+      <c r="S44" s="14"/>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A45" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B45" s="10"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="I45" s="13"/>
+      <c r="J45" s="13"/>
+      <c r="K45" s="13"/>
+      <c r="L45" s="13"/>
+      <c r="M45" s="13"/>
+      <c r="N45" s="14"/>
+      <c r="O45" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="P45" s="13"/>
+      <c r="Q45" s="14"/>
+      <c r="R45" s="12">
+        <v>833</v>
+      </c>
+      <c r="S45" s="14"/>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A46" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B46" s="10"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="E46" s="10"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="11"/>
+      <c r="H46" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="I46" s="13"/>
+      <c r="J46" s="13"/>
+      <c r="K46" s="13"/>
+      <c r="L46" s="13"/>
+      <c r="M46" s="13"/>
+      <c r="N46" s="14"/>
+      <c r="O46" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="P46" s="13"/>
+      <c r="Q46" s="14"/>
+      <c r="R46" s="12">
+        <v>3139</v>
+      </c>
+      <c r="S46" s="14"/>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A47" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B47" s="10"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="E47" s="10"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="I47" s="13"/>
+      <c r="J47" s="13"/>
+      <c r="K47" s="13"/>
+      <c r="L47" s="13"/>
+      <c r="M47" s="13"/>
+      <c r="N47" s="14"/>
+      <c r="O47" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="P47" s="13"/>
+      <c r="Q47" s="14"/>
+      <c r="R47" s="12">
+        <v>3139</v>
+      </c>
+      <c r="S47" s="14"/>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A48" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B48" s="10"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E48" s="10"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="I48" s="13"/>
+      <c r="J48" s="13"/>
+      <c r="K48" s="13"/>
+      <c r="L48" s="13"/>
+      <c r="M48" s="13"/>
+      <c r="N48" s="14"/>
+      <c r="O48" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="P48" s="13"/>
+      <c r="Q48" s="14"/>
+      <c r="R48" s="12">
+        <v>120289</v>
+      </c>
+      <c r="S48" s="14"/>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A49" s="9">
+        <v>110</v>
+      </c>
+      <c r="B49" s="10"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="E49" s="10"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="11"/>
+      <c r="H49" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I49" s="13"/>
+      <c r="J49" s="13"/>
+      <c r="K49" s="13"/>
+      <c r="L49" s="13"/>
+      <c r="M49" s="13"/>
+      <c r="N49" s="14"/>
+      <c r="O49" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="P49" s="13"/>
+      <c r="Q49" s="14"/>
+      <c r="R49" s="12">
+        <v>844</v>
+      </c>
+      <c r="S49" s="14"/>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A50" s="9">
+        <v>110</v>
+      </c>
+      <c r="B50" s="10"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="E50" s="10"/>
+      <c r="F50" s="10"/>
+      <c r="G50" s="11"/>
+      <c r="H50" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I50" s="13"/>
+      <c r="J50" s="13"/>
+      <c r="K50" s="13"/>
+      <c r="L50" s="13"/>
+      <c r="M50" s="13"/>
+      <c r="N50" s="14"/>
+      <c r="O50" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="P50" s="13"/>
+      <c r="Q50" s="14"/>
+      <c r="R50" s="12">
+        <v>844</v>
+      </c>
+      <c r="S50" s="14"/>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A51" s="9">
+        <v>110</v>
+      </c>
+      <c r="B51" s="10"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="E51" s="10"/>
+      <c r="F51" s="10"/>
+      <c r="G51" s="11"/>
+      <c r="H51" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I51" s="13"/>
+      <c r="J51" s="13"/>
+      <c r="K51" s="13"/>
+      <c r="L51" s="13"/>
+      <c r="M51" s="13"/>
+      <c r="N51" s="14"/>
+      <c r="O51" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="P51" s="13"/>
+      <c r="Q51" s="14"/>
+      <c r="R51" s="12">
+        <v>844</v>
+      </c>
+      <c r="S51" s="14"/>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A52" s="9">
+        <v>110</v>
+      </c>
+      <c r="B52" s="10"/>
+      <c r="C52" s="11"/>
+      <c r="D52" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="E52" s="10"/>
+      <c r="F52" s="10"/>
+      <c r="G52" s="11"/>
+      <c r="H52" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I52" s="13"/>
+      <c r="J52" s="13"/>
+      <c r="K52" s="13"/>
+      <c r="L52" s="13"/>
+      <c r="M52" s="13"/>
+      <c r="N52" s="14"/>
+      <c r="O52" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="P52" s="13"/>
+      <c r="Q52" s="14"/>
+      <c r="R52" s="12">
+        <v>844</v>
+      </c>
+      <c r="S52" s="14"/>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A53" s="9">
+        <v>110</v>
+      </c>
+      <c r="B53" s="10"/>
+      <c r="C53" s="11"/>
+      <c r="D53" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="E53" s="10"/>
+      <c r="F53" s="10"/>
+      <c r="G53" s="11"/>
+      <c r="H53" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I53" s="13"/>
+      <c r="J53" s="13"/>
+      <c r="K53" s="13"/>
+      <c r="L53" s="13"/>
+      <c r="M53" s="13"/>
+      <c r="N53" s="14"/>
+      <c r="O53" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="P53" s="13"/>
+      <c r="Q53" s="14"/>
+      <c r="R53" s="12">
+        <v>844</v>
+      </c>
+      <c r="S53" s="14"/>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A54" s="9">
+        <v>110</v>
+      </c>
+      <c r="B54" s="10"/>
+      <c r="C54" s="11"/>
+      <c r="D54" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="E54" s="10"/>
+      <c r="F54" s="10"/>
+      <c r="G54" s="11"/>
+      <c r="H54" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I54" s="13"/>
+      <c r="J54" s="13"/>
+      <c r="K54" s="13"/>
+      <c r="L54" s="13"/>
+      <c r="M54" s="13"/>
+      <c r="N54" s="14"/>
+      <c r="O54" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="P54" s="13"/>
+      <c r="Q54" s="14"/>
+      <c r="R54" s="12">
+        <v>844</v>
+      </c>
+      <c r="S54" s="14"/>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A55" s="9">
+        <v>110</v>
+      </c>
+      <c r="B55" s="10"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="E55" s="10"/>
+      <c r="F55" s="10"/>
+      <c r="G55" s="11"/>
+      <c r="H55" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I55" s="13"/>
+      <c r="J55" s="13"/>
+      <c r="K55" s="13"/>
+      <c r="L55" s="13"/>
+      <c r="M55" s="13"/>
+      <c r="N55" s="14"/>
+      <c r="O55" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="P55" s="13"/>
+      <c r="Q55" s="14"/>
+      <c r="R55" s="12">
+        <v>844</v>
+      </c>
+      <c r="S55" s="14"/>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A56" s="9">
+        <v>110</v>
+      </c>
+      <c r="B56" s="10"/>
+      <c r="C56" s="11"/>
+      <c r="D56" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="E56" s="10"/>
+      <c r="F56" s="10"/>
+      <c r="G56" s="11"/>
+      <c r="H56" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I56" s="13"/>
+      <c r="J56" s="13"/>
+      <c r="K56" s="13"/>
+      <c r="L56" s="13"/>
+      <c r="M56" s="13"/>
+      <c r="N56" s="14"/>
+      <c r="O56" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="P56" s="13"/>
+      <c r="Q56" s="14"/>
+      <c r="R56" s="12">
+        <v>844</v>
+      </c>
+      <c r="S56" s="14"/>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A57" s="9">
+        <v>510</v>
+      </c>
+      <c r="B57" s="10"/>
+      <c r="C57" s="11"/>
+      <c r="D57" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="E57" s="10"/>
+      <c r="F57" s="10"/>
+      <c r="G57" s="11"/>
+      <c r="H57" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I57" s="13"/>
+      <c r="J57" s="13"/>
+      <c r="K57" s="13"/>
+      <c r="L57" s="13"/>
+      <c r="M57" s="13"/>
+      <c r="N57" s="14"/>
+      <c r="O57" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="P57" s="13"/>
+      <c r="Q57" s="14"/>
+      <c r="R57" s="12">
+        <v>1400280</v>
+      </c>
+      <c r="S57" s="14"/>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A58" s="9">
+        <v>510</v>
+      </c>
+      <c r="B58" s="10"/>
+      <c r="C58" s="11"/>
+      <c r="D58" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="E58" s="10"/>
+      <c r="F58" s="10"/>
+      <c r="G58" s="11"/>
+      <c r="H58" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I58" s="13"/>
+      <c r="J58" s="13"/>
+      <c r="K58" s="13"/>
+      <c r="L58" s="13"/>
+      <c r="M58" s="13"/>
+      <c r="N58" s="14"/>
+      <c r="O58" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="P58" s="13"/>
+      <c r="Q58" s="14"/>
+      <c r="R58" s="12">
+        <v>1400280</v>
+      </c>
+      <c r="S58" s="14"/>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A59" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B59" s="10"/>
+      <c r="C59" s="11"/>
+      <c r="D59" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="E59" s="10"/>
+      <c r="F59" s="10"/>
+      <c r="G59" s="11"/>
+      <c r="H59" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I59" s="13"/>
+      <c r="J59" s="13"/>
+      <c r="K59" s="13"/>
+      <c r="L59" s="13"/>
+      <c r="M59" s="13"/>
+      <c r="N59" s="14"/>
+      <c r="O59" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="P59" s="13"/>
+      <c r="Q59" s="14"/>
+      <c r="R59" s="12">
+        <v>436191</v>
+      </c>
+      <c r="S59" s="14"/>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A60" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B60" s="10"/>
+      <c r="C60" s="11"/>
+      <c r="D60" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="E60" s="10"/>
+      <c r="F60" s="10"/>
+      <c r="G60" s="11"/>
+      <c r="H60" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I60" s="13"/>
+      <c r="J60" s="13"/>
+      <c r="K60" s="13"/>
+      <c r="L60" s="13"/>
+      <c r="M60" s="13"/>
+      <c r="N60" s="14"/>
+      <c r="O60" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="P60" s="13"/>
+      <c r="Q60" s="14"/>
+      <c r="R60" s="12">
+        <v>436191</v>
+      </c>
+      <c r="S60" s="14"/>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A61" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B61" s="10"/>
+      <c r="C61" s="11"/>
+      <c r="D61" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="E61" s="10"/>
+      <c r="F61" s="10"/>
+      <c r="G61" s="11"/>
+      <c r="H61" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I61" s="13"/>
+      <c r="J61" s="13"/>
+      <c r="K61" s="13"/>
+      <c r="L61" s="13"/>
+      <c r="M61" s="13"/>
+      <c r="N61" s="14"/>
+      <c r="O61" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="P61" s="13"/>
+      <c r="Q61" s="14"/>
+      <c r="R61" s="12">
+        <v>3316</v>
+      </c>
+      <c r="S61" s="14"/>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A62" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B62" s="10"/>
+      <c r="C62" s="11"/>
+      <c r="D62" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="E62" s="10"/>
+      <c r="F62" s="10"/>
+      <c r="G62" s="11"/>
+      <c r="H62" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I62" s="13"/>
+      <c r="J62" s="13"/>
+      <c r="K62" s="13"/>
+      <c r="L62" s="13"/>
+      <c r="M62" s="13"/>
+      <c r="N62" s="14"/>
+      <c r="O62" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="P62" s="13"/>
+      <c r="Q62" s="14"/>
+      <c r="R62" s="12">
+        <v>3316</v>
+      </c>
+      <c r="S62" s="14"/>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A63" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B63" s="10"/>
+      <c r="C63" s="11"/>
+      <c r="D63" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E63" s="10"/>
+      <c r="F63" s="10"/>
+      <c r="G63" s="11"/>
+      <c r="H63" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I63" s="13"/>
+      <c r="J63" s="13"/>
+      <c r="K63" s="13"/>
+      <c r="L63" s="13"/>
+      <c r="M63" s="13"/>
+      <c r="N63" s="14"/>
+      <c r="O63" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="P63" s="13"/>
+      <c r="Q63" s="14"/>
+      <c r="R63" s="12">
+        <v>163751</v>
+      </c>
+      <c r="S63" s="14"/>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A64" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B64" s="10"/>
+      <c r="C64" s="11"/>
+      <c r="D64" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="E64" s="10"/>
+      <c r="F64" s="10"/>
+      <c r="G64" s="11"/>
+      <c r="H64" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I64" s="13"/>
+      <c r="J64" s="13"/>
+      <c r="K64" s="13"/>
+      <c r="L64" s="13"/>
+      <c r="M64" s="13"/>
+      <c r="N64" s="14"/>
+      <c r="O64" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="P64" s="13"/>
+      <c r="Q64" s="14"/>
+      <c r="R64" s="12">
+        <v>693108</v>
+      </c>
+      <c r="S64" s="14"/>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A65" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B65" s="10"/>
+      <c r="C65" s="11"/>
+      <c r="D65" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="E65" s="10"/>
+      <c r="F65" s="10"/>
+      <c r="G65" s="11"/>
+      <c r="H65" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I65" s="13"/>
+      <c r="J65" s="13"/>
+      <c r="K65" s="13"/>
+      <c r="L65" s="13"/>
+      <c r="M65" s="13"/>
+      <c r="N65" s="14"/>
+      <c r="O65" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="P65" s="13"/>
+      <c r="Q65" s="14"/>
+      <c r="R65" s="12">
+        <v>693108</v>
+      </c>
+      <c r="S65" s="14"/>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A66" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B66" s="10"/>
+      <c r="C66" s="11"/>
+      <c r="D66" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="E66" s="10"/>
+      <c r="F66" s="10"/>
+      <c r="G66" s="11"/>
+      <c r="H66" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I66" s="13"/>
+      <c r="J66" s="13"/>
+      <c r="K66" s="13"/>
+      <c r="L66" s="13"/>
+      <c r="M66" s="13"/>
+      <c r="N66" s="14"/>
+      <c r="O66" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="P66" s="13"/>
+      <c r="Q66" s="14"/>
+      <c r="R66" s="12">
+        <v>693108</v>
+      </c>
+      <c r="S66" s="14"/>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A67" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B67" s="10"/>
+      <c r="C67" s="11"/>
+      <c r="D67" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="E67" s="10"/>
+      <c r="F67" s="10"/>
+      <c r="G67" s="11"/>
+      <c r="H67" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I67" s="13"/>
+      <c r="J67" s="13"/>
+      <c r="K67" s="13"/>
+      <c r="L67" s="13"/>
+      <c r="M67" s="13"/>
+      <c r="N67" s="14"/>
+      <c r="O67" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="P67" s="13"/>
+      <c r="Q67" s="14"/>
+      <c r="R67" s="12">
+        <v>693108</v>
+      </c>
+      <c r="S67" s="14"/>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A68" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B68" s="10"/>
+      <c r="C68" s="11"/>
+      <c r="D68" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="E68" s="10"/>
+      <c r="F68" s="10"/>
+      <c r="G68" s="11"/>
+      <c r="H68" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I68" s="13"/>
+      <c r="J68" s="13"/>
+      <c r="K68" s="13"/>
+      <c r="L68" s="13"/>
+      <c r="M68" s="13"/>
+      <c r="N68" s="14"/>
+      <c r="O68" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="P68" s="13"/>
+      <c r="Q68" s="14"/>
+      <c r="R68" s="12">
+        <v>18834045</v>
+      </c>
+      <c r="S68" s="14"/>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A69" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B69" s="10"/>
+      <c r="C69" s="11"/>
+      <c r="D69" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E69" s="10"/>
+      <c r="F69" s="10"/>
+      <c r="G69" s="11"/>
+      <c r="H69" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I69" s="13"/>
+      <c r="J69" s="13"/>
+      <c r="K69" s="13"/>
+      <c r="L69" s="13"/>
+      <c r="M69" s="13"/>
+      <c r="N69" s="14"/>
+      <c r="O69" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="P69" s="13"/>
+      <c r="Q69" s="14"/>
+      <c r="R69" s="12">
+        <v>18834045</v>
+      </c>
+      <c r="S69" s="14"/>
+    </row>
+    <row r="70" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A70" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B70" s="10"/>
+      <c r="C70" s="11"/>
+      <c r="D70" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="E70" s="10"/>
+      <c r="F70" s="10"/>
+      <c r="G70" s="11"/>
+      <c r="H70" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I70" s="13"/>
+      <c r="J70" s="13"/>
+      <c r="K70" s="13"/>
+      <c r="L70" s="13"/>
+      <c r="M70" s="13"/>
+      <c r="N70" s="14"/>
+      <c r="O70" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="P70" s="13"/>
+      <c r="Q70" s="14"/>
+      <c r="R70" s="12">
+        <v>18834045</v>
+      </c>
+      <c r="S70" s="14"/>
+    </row>
+    <row r="71" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A71" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B71" s="10"/>
+      <c r="C71" s="11"/>
+      <c r="D71" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="E71" s="10"/>
+      <c r="F71" s="10"/>
+      <c r="G71" s="11"/>
+      <c r="H71" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I71" s="13"/>
+      <c r="J71" s="13"/>
+      <c r="K71" s="13"/>
+      <c r="L71" s="13"/>
+      <c r="M71" s="13"/>
+      <c r="N71" s="14"/>
+      <c r="O71" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="P71" s="13"/>
+      <c r="Q71" s="14"/>
+      <c r="R71" s="12">
+        <v>18834045</v>
+      </c>
+      <c r="S71" s="14"/>
+    </row>
+    <row r="72" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A72" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B72" s="10"/>
+      <c r="C72" s="11"/>
+      <c r="D72" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="E72" s="10"/>
+      <c r="F72" s="10"/>
+      <c r="G72" s="11"/>
+      <c r="H72" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I72" s="13"/>
+      <c r="J72" s="13"/>
+      <c r="K72" s="13"/>
+      <c r="L72" s="13"/>
+      <c r="M72" s="13"/>
+      <c r="N72" s="14"/>
+      <c r="O72" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="P72" s="13"/>
+      <c r="Q72" s="14"/>
+      <c r="R72" s="12">
+        <v>18834045</v>
+      </c>
+      <c r="S72" s="14"/>
+    </row>
+    <row r="73" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A73" s="9">
+        <v>0</v>
+      </c>
+      <c r="B73" s="10"/>
+      <c r="C73" s="11"/>
+      <c r="D73" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="E73" s="10"/>
+      <c r="F73" s="10"/>
+      <c r="G73" s="11"/>
+      <c r="H73" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I73" s="13"/>
+      <c r="J73" s="13"/>
+      <c r="K73" s="13"/>
+      <c r="L73" s="13"/>
+      <c r="M73" s="13"/>
+      <c r="N73" s="14"/>
+      <c r="O73" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="P73" s="13"/>
+      <c r="Q73" s="14"/>
+      <c r="R73" s="12">
+        <v>1157685</v>
+      </c>
+      <c r="S73" s="14"/>
+    </row>
+    <row r="74" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A74" s="9">
+        <v>0</v>
+      </c>
+      <c r="B74" s="10"/>
+      <c r="C74" s="11"/>
+      <c r="D74" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="E74" s="10"/>
+      <c r="F74" s="10"/>
+      <c r="G74" s="11"/>
+      <c r="H74" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I74" s="13"/>
+      <c r="J74" s="13"/>
+      <c r="K74" s="13"/>
+      <c r="L74" s="13"/>
+      <c r="M74" s="13"/>
+      <c r="N74" s="14"/>
+      <c r="O74" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="P74" s="13"/>
+      <c r="Q74" s="14"/>
+      <c r="R74" s="12">
+        <v>1157685</v>
+      </c>
+      <c r="S74" s="14"/>
+    </row>
+    <row r="75" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A75" s="9">
+        <v>120</v>
+      </c>
+      <c r="B75" s="10"/>
+      <c r="C75" s="11"/>
+      <c r="D75" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="E75" s="10"/>
+      <c r="F75" s="10"/>
+      <c r="G75" s="11"/>
+      <c r="H75" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I75" s="13"/>
+      <c r="J75" s="13"/>
+      <c r="K75" s="13"/>
+      <c r="L75" s="13"/>
+      <c r="M75" s="13"/>
+      <c r="N75" s="14"/>
+      <c r="O75" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="P75" s="13"/>
+      <c r="Q75" s="14"/>
+      <c r="R75" s="12">
+        <v>303844</v>
+      </c>
+      <c r="S75" s="14"/>
+    </row>
+    <row r="76" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A76" s="9">
+        <v>120</v>
+      </c>
+      <c r="B76" s="10"/>
+      <c r="C76" s="11"/>
+      <c r="D76" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="E76" s="10"/>
+      <c r="F76" s="10"/>
+      <c r="G76" s="11"/>
+      <c r="H76" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I76" s="13"/>
+      <c r="J76" s="13"/>
+      <c r="K76" s="13"/>
+      <c r="L76" s="13"/>
+      <c r="M76" s="13"/>
+      <c r="N76" s="14"/>
+      <c r="O76" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="P76" s="13"/>
+      <c r="Q76" s="14"/>
+      <c r="R76" s="12">
+        <v>303844</v>
+      </c>
+      <c r="S76" s="14"/>
+    </row>
+    <row r="77" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A77" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B77" s="10"/>
+      <c r="C77" s="11"/>
+      <c r="D77" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E77" s="10"/>
+      <c r="F77" s="10"/>
+      <c r="G77" s="11"/>
+      <c r="H77" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I77" s="13"/>
+      <c r="J77" s="13"/>
+      <c r="K77" s="13"/>
+      <c r="L77" s="13"/>
+      <c r="M77" s="13"/>
+      <c r="N77" s="14"/>
+      <c r="O77" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="P77" s="13"/>
+      <c r="Q77" s="14"/>
+      <c r="R77" s="12">
+        <v>50</v>
+      </c>
+      <c r="S77" s="14"/>
+    </row>
+    <row r="78" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A78" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B78" s="10"/>
+      <c r="C78" s="11"/>
+      <c r="D78" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E78" s="10"/>
+      <c r="F78" s="10"/>
+      <c r="G78" s="11"/>
+      <c r="H78" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I78" s="13"/>
+      <c r="J78" s="13"/>
+      <c r="K78" s="13"/>
+      <c r="L78" s="13"/>
+      <c r="M78" s="13"/>
+      <c r="N78" s="14"/>
+      <c r="O78" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="P78" s="13"/>
+      <c r="Q78" s="14"/>
+      <c r="R78" s="12">
+        <v>2177</v>
+      </c>
+      <c r="S78" s="14"/>
+    </row>
+    <row r="79" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A79" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B79" s="10"/>
+      <c r="C79" s="11"/>
+      <c r="D79" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E79" s="10"/>
+      <c r="F79" s="10"/>
+      <c r="G79" s="11"/>
+      <c r="H79" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I79" s="13"/>
+      <c r="J79" s="13"/>
+      <c r="K79" s="13"/>
+      <c r="L79" s="13"/>
+      <c r="M79" s="13"/>
+      <c r="N79" s="14"/>
+      <c r="O79" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="P79" s="13"/>
+      <c r="Q79" s="14"/>
+      <c r="R79" s="12">
+        <v>9841243</v>
+      </c>
+      <c r="S79" s="14"/>
+    </row>
+    <row r="80" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A80" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B80" s="10"/>
+      <c r="C80" s="11"/>
+      <c r="D80" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E80" s="10"/>
+      <c r="F80" s="10"/>
+      <c r="G80" s="11"/>
+      <c r="H80" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="I80" s="13"/>
+      <c r="J80" s="13"/>
+      <c r="K80" s="13"/>
+      <c r="L80" s="13"/>
+      <c r="M80" s="13"/>
+      <c r="N80" s="14"/>
+      <c r="O80" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="P80" s="13"/>
+      <c r="Q80" s="14"/>
+      <c r="R80" s="12">
+        <v>1753</v>
+      </c>
+      <c r="S80" s="14"/>
+    </row>
+    <row r="81" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A81" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B81" s="10"/>
+      <c r="C81" s="11"/>
+      <c r="D81" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E81" s="10"/>
+      <c r="F81" s="10"/>
+      <c r="G81" s="11"/>
+      <c r="H81" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="I81" s="13"/>
+      <c r="J81" s="13"/>
+      <c r="K81" s="13"/>
+      <c r="L81" s="13"/>
+      <c r="M81" s="13"/>
+      <c r="N81" s="14"/>
+      <c r="O81" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="P81" s="13"/>
+      <c r="Q81" s="14"/>
+      <c r="R81" s="12">
+        <v>3625</v>
+      </c>
+      <c r="S81" s="14"/>
+    </row>
+    <row r="82" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A82" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B82" s="10"/>
+      <c r="C82" s="11"/>
+      <c r="D82" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="E82" s="10"/>
+      <c r="F82" s="10"/>
+      <c r="G82" s="11"/>
+      <c r="H82" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="I82" s="13"/>
+      <c r="J82" s="13"/>
+      <c r="K82" s="13"/>
+      <c r="L82" s="13"/>
+      <c r="M82" s="13"/>
+      <c r="N82" s="14"/>
+      <c r="O82" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="P82" s="13"/>
+      <c r="Q82" s="14"/>
+      <c r="R82" s="12">
+        <v>314</v>
+      </c>
+      <c r="S82" s="14"/>
+    </row>
+    <row r="83" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A83" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B83" s="10"/>
+      <c r="C83" s="11"/>
+      <c r="D83" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E83" s="10"/>
+      <c r="F83" s="10"/>
+      <c r="G83" s="11"/>
+      <c r="H83" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="I83" s="13"/>
+      <c r="J83" s="13"/>
+      <c r="K83" s="13"/>
+      <c r="L83" s="13"/>
+      <c r="M83" s="13"/>
+      <c r="N83" s="14"/>
+      <c r="O83" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="P83" s="13"/>
+      <c r="Q83" s="14"/>
+      <c r="R83" s="12">
+        <v>314</v>
+      </c>
+      <c r="S83" s="14"/>
+    </row>
+    <row r="84" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A84" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B84" s="10"/>
+      <c r="C84" s="11"/>
+      <c r="D84" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="E84" s="10"/>
+      <c r="F84" s="10"/>
+      <c r="G84" s="11"/>
+      <c r="H84" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="I84" s="13"/>
+      <c r="J84" s="13"/>
+      <c r="K84" s="13"/>
+      <c r="L84" s="13"/>
+      <c r="M84" s="13"/>
+      <c r="N84" s="14"/>
+      <c r="O84" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="P84" s="13"/>
+      <c r="Q84" s="14"/>
+      <c r="R84" s="12">
+        <v>5671</v>
+      </c>
+      <c r="S84" s="14"/>
+    </row>
+    <row r="85" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A85" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B85" s="10"/>
+      <c r="C85" s="11"/>
+      <c r="D85" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E85" s="10"/>
+      <c r="F85" s="10"/>
+      <c r="G85" s="11"/>
+      <c r="H85" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="I85" s="13"/>
+      <c r="J85" s="13"/>
+      <c r="K85" s="13"/>
+      <c r="L85" s="13"/>
+      <c r="M85" s="13"/>
+      <c r="N85" s="14"/>
+      <c r="O85" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="P85" s="13"/>
+      <c r="Q85" s="14"/>
+      <c r="R85" s="12">
+        <v>5671</v>
+      </c>
+      <c r="S85" s="14"/>
+    </row>
+    <row r="86" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A86" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="B86" s="19"/>
+      <c r="C86" s="20"/>
+      <c r="D86" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E86" s="10"/>
+      <c r="F86" s="10"/>
+      <c r="G86" s="11"/>
+      <c r="H86" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="I86" s="13"/>
+      <c r="J86" s="13"/>
+      <c r="K86" s="13"/>
+      <c r="L86" s="13"/>
+      <c r="M86" s="13"/>
+      <c r="N86" s="14"/>
+      <c r="O86" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="P86" s="13"/>
+      <c r="Q86" s="14"/>
+      <c r="R86" s="12">
+        <v>4172</v>
+      </c>
+      <c r="S86" s="14"/>
+    </row>
+    <row r="87" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A87" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B87" s="10"/>
+      <c r="C87" s="11"/>
+      <c r="D87" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="E87" s="10"/>
+      <c r="F87" s="10"/>
+      <c r="G87" s="11"/>
+      <c r="H87" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="I87" s="13"/>
+      <c r="J87" s="13"/>
+      <c r="K87" s="13"/>
+      <c r="L87" s="13"/>
+      <c r="M87" s="13"/>
+      <c r="N87" s="14"/>
+      <c r="O87" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="P87" s="13"/>
+      <c r="Q87" s="14"/>
+      <c r="R87" s="12">
         <v>286</v>
       </c>
-      <c r="S32" s="14"/>
+      <c r="S87" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="160">
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="D31:G31"/>
-    <mergeCell ref="H31:N31"/>
-    <mergeCell ref="O31:Q31"/>
+  <mergeCells count="435">
+    <mergeCell ref="A84:C84"/>
+    <mergeCell ref="D84:G84"/>
+    <mergeCell ref="H84:N84"/>
+    <mergeCell ref="O84:Q84"/>
+    <mergeCell ref="R84:S84"/>
+    <mergeCell ref="A75:C75"/>
+    <mergeCell ref="D75:G75"/>
+    <mergeCell ref="H75:N75"/>
+    <mergeCell ref="O75:Q75"/>
+    <mergeCell ref="R75:S75"/>
+    <mergeCell ref="A82:C82"/>
+    <mergeCell ref="D82:G82"/>
+    <mergeCell ref="H82:N82"/>
+    <mergeCell ref="O82:Q82"/>
+    <mergeCell ref="R82:S82"/>
+    <mergeCell ref="A70:C70"/>
+    <mergeCell ref="D70:G70"/>
+    <mergeCell ref="H70:N70"/>
+    <mergeCell ref="O70:Q70"/>
+    <mergeCell ref="R70:S70"/>
+    <mergeCell ref="A71:C71"/>
+    <mergeCell ref="D71:G71"/>
+    <mergeCell ref="H71:N71"/>
+    <mergeCell ref="O71:Q71"/>
+    <mergeCell ref="R71:S71"/>
+    <mergeCell ref="R66:S66"/>
+    <mergeCell ref="A68:C68"/>
+    <mergeCell ref="D68:G68"/>
+    <mergeCell ref="H68:N68"/>
+    <mergeCell ref="O68:Q68"/>
+    <mergeCell ref="R68:S68"/>
+    <mergeCell ref="A69:C69"/>
+    <mergeCell ref="D69:G69"/>
+    <mergeCell ref="H69:N69"/>
+    <mergeCell ref="O69:Q69"/>
+    <mergeCell ref="R69:S69"/>
+    <mergeCell ref="A59:C59"/>
+    <mergeCell ref="D59:G59"/>
+    <mergeCell ref="H59:N59"/>
+    <mergeCell ref="O59:Q59"/>
+    <mergeCell ref="R59:S59"/>
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="D61:G61"/>
+    <mergeCell ref="H61:N61"/>
+    <mergeCell ref="O61:Q61"/>
+    <mergeCell ref="R61:S61"/>
+    <mergeCell ref="A55:C55"/>
+    <mergeCell ref="D55:G55"/>
+    <mergeCell ref="H55:N55"/>
+    <mergeCell ref="O55:Q55"/>
+    <mergeCell ref="R55:S55"/>
+    <mergeCell ref="A57:C57"/>
+    <mergeCell ref="D57:G57"/>
+    <mergeCell ref="H57:N57"/>
+    <mergeCell ref="O57:Q57"/>
+    <mergeCell ref="R57:S57"/>
+    <mergeCell ref="A53:C53"/>
+    <mergeCell ref="D53:G53"/>
+    <mergeCell ref="H53:N53"/>
+    <mergeCell ref="O53:Q53"/>
+    <mergeCell ref="R53:S53"/>
+    <mergeCell ref="A54:C54"/>
+    <mergeCell ref="D54:G54"/>
+    <mergeCell ref="H54:N54"/>
+    <mergeCell ref="O54:Q54"/>
+    <mergeCell ref="R54:S54"/>
+    <mergeCell ref="A51:C51"/>
+    <mergeCell ref="D51:G51"/>
+    <mergeCell ref="H51:N51"/>
+    <mergeCell ref="O51:Q51"/>
+    <mergeCell ref="R51:S51"/>
+    <mergeCell ref="A52:C52"/>
+    <mergeCell ref="D52:G52"/>
+    <mergeCell ref="H52:N52"/>
+    <mergeCell ref="O52:Q52"/>
+    <mergeCell ref="R52:S52"/>
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="D49:G49"/>
+    <mergeCell ref="H49:N49"/>
+    <mergeCell ref="O49:Q49"/>
+    <mergeCell ref="R49:S49"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="D50:G50"/>
+    <mergeCell ref="H50:N50"/>
+    <mergeCell ref="O50:Q50"/>
+    <mergeCell ref="R50:S50"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="D43:G43"/>
+    <mergeCell ref="H43:N43"/>
+    <mergeCell ref="O43:Q43"/>
+    <mergeCell ref="R43:S43"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="D46:G46"/>
+    <mergeCell ref="H46:N46"/>
+    <mergeCell ref="O46:Q46"/>
+    <mergeCell ref="R46:S46"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="D41:G41"/>
+    <mergeCell ref="H41:N41"/>
+    <mergeCell ref="O41:Q41"/>
+    <mergeCell ref="R41:S41"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="D42:G42"/>
+    <mergeCell ref="H42:N42"/>
+    <mergeCell ref="O42:Q42"/>
+    <mergeCell ref="R42:S42"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="D35:G35"/>
+    <mergeCell ref="H35:N35"/>
+    <mergeCell ref="O35:Q35"/>
+    <mergeCell ref="R35:S35"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="D39:G39"/>
+    <mergeCell ref="H39:N39"/>
+    <mergeCell ref="O39:Q39"/>
+    <mergeCell ref="R39:S39"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="D36:G36"/>
+    <mergeCell ref="H36:N36"/>
+    <mergeCell ref="O36:Q36"/>
+    <mergeCell ref="R36:S36"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="D37:G37"/>
+    <mergeCell ref="H37:N37"/>
+    <mergeCell ref="O37:Q37"/>
+    <mergeCell ref="R37:S37"/>
     <mergeCell ref="R31:S31"/>
     <mergeCell ref="A32:C32"/>
     <mergeCell ref="D32:G32"/>
     <mergeCell ref="H32:N32"/>
     <mergeCell ref="O32:Q32"/>
     <mergeCell ref="R32:S32"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="D29:G29"/>
-    <mergeCell ref="H29:N29"/>
-    <mergeCell ref="O29:Q29"/>
-    <mergeCell ref="R29:S29"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="D30:G30"/>
-    <mergeCell ref="H30:N30"/>
-    <mergeCell ref="O30:Q30"/>
-    <mergeCell ref="R30:S30"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="H27:N27"/>
-    <mergeCell ref="O27:Q27"/>
-    <mergeCell ref="R27:S27"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="D33:G33"/>
+    <mergeCell ref="H33:N33"/>
+    <mergeCell ref="O33:Q33"/>
+    <mergeCell ref="R33:S33"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="H26:N26"/>
+    <mergeCell ref="O26:Q26"/>
+    <mergeCell ref="R26:S26"/>
     <mergeCell ref="A28:C28"/>
     <mergeCell ref="D28:G28"/>
     <mergeCell ref="H28:N28"/>
     <mergeCell ref="O28:Q28"/>
     <mergeCell ref="R28:S28"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="D23:G23"/>
+    <mergeCell ref="H23:N23"/>
+    <mergeCell ref="O23:Q23"/>
+    <mergeCell ref="R23:S23"/>
     <mergeCell ref="A25:C25"/>
     <mergeCell ref="D25:G25"/>
     <mergeCell ref="H25:N25"/>
     <mergeCell ref="O25:Q25"/>
     <mergeCell ref="R25:S25"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="H26:N26"/>
-    <mergeCell ref="O26:Q26"/>
-    <mergeCell ref="R26:S26"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="D23:G23"/>
-    <mergeCell ref="H23:N23"/>
-    <mergeCell ref="O23:Q23"/>
-    <mergeCell ref="R23:S23"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="D24:G24"/>
-    <mergeCell ref="H24:N24"/>
-    <mergeCell ref="O24:Q24"/>
-    <mergeCell ref="R24:S24"/>
     <mergeCell ref="A21:C21"/>
     <mergeCell ref="D21:G21"/>
     <mergeCell ref="H21:N21"/>
@@ -1917,16 +3870,13 @@
     <mergeCell ref="H8:N8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="R8:S8"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="H5:N5"/>
-    <mergeCell ref="O5:Q5"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="H6:N6"/>
     <mergeCell ref="O6:Q6"/>
     <mergeCell ref="R6:S6"/>
+    <mergeCell ref="A87:C87"/>
+    <mergeCell ref="D87:G87"/>
+    <mergeCell ref="H87:N87"/>
+    <mergeCell ref="O87:Q87"/>
+    <mergeCell ref="R87:S87"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="D3:G3"/>
     <mergeCell ref="H3:N3"/>
@@ -1937,6 +3887,177 @@
     <mergeCell ref="H4:N4"/>
     <mergeCell ref="O4:Q4"/>
     <mergeCell ref="R4:S4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="H5:N5"/>
+    <mergeCell ref="O5:Q5"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="H6:N6"/>
+    <mergeCell ref="A85:C85"/>
+    <mergeCell ref="D85:G85"/>
+    <mergeCell ref="H85:N85"/>
+    <mergeCell ref="O85:Q85"/>
+    <mergeCell ref="R85:S85"/>
+    <mergeCell ref="A86:C86"/>
+    <mergeCell ref="D86:G86"/>
+    <mergeCell ref="H86:N86"/>
+    <mergeCell ref="O86:Q86"/>
+    <mergeCell ref="R86:S86"/>
+    <mergeCell ref="A81:C81"/>
+    <mergeCell ref="D81:G81"/>
+    <mergeCell ref="H81:N81"/>
+    <mergeCell ref="O81:Q81"/>
+    <mergeCell ref="R81:S81"/>
+    <mergeCell ref="A83:C83"/>
+    <mergeCell ref="D83:G83"/>
+    <mergeCell ref="H83:N83"/>
+    <mergeCell ref="O83:Q83"/>
+    <mergeCell ref="R83:S83"/>
+    <mergeCell ref="A80:C80"/>
+    <mergeCell ref="D80:G80"/>
+    <mergeCell ref="H80:N80"/>
+    <mergeCell ref="O80:Q80"/>
+    <mergeCell ref="R80:S80"/>
+    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="D78:G78"/>
+    <mergeCell ref="H78:N78"/>
+    <mergeCell ref="O78:Q78"/>
+    <mergeCell ref="R78:S78"/>
+    <mergeCell ref="A79:C79"/>
+    <mergeCell ref="D79:G79"/>
+    <mergeCell ref="H79:N79"/>
+    <mergeCell ref="O79:Q79"/>
+    <mergeCell ref="R79:S79"/>
+    <mergeCell ref="A76:C76"/>
+    <mergeCell ref="D76:G76"/>
+    <mergeCell ref="H76:N76"/>
+    <mergeCell ref="O76:Q76"/>
+    <mergeCell ref="R76:S76"/>
+    <mergeCell ref="A77:C77"/>
+    <mergeCell ref="D77:G77"/>
+    <mergeCell ref="H77:N77"/>
+    <mergeCell ref="O77:Q77"/>
+    <mergeCell ref="R77:S77"/>
+    <mergeCell ref="A72:C72"/>
+    <mergeCell ref="D72:G72"/>
+    <mergeCell ref="H72:N72"/>
+    <mergeCell ref="O72:Q72"/>
+    <mergeCell ref="R72:S72"/>
+    <mergeCell ref="A74:C74"/>
+    <mergeCell ref="D74:G74"/>
+    <mergeCell ref="H74:N74"/>
+    <mergeCell ref="O74:Q74"/>
+    <mergeCell ref="R74:S74"/>
+    <mergeCell ref="A73:C73"/>
+    <mergeCell ref="D73:G73"/>
+    <mergeCell ref="H73:N73"/>
+    <mergeCell ref="O73:Q73"/>
+    <mergeCell ref="R73:S73"/>
+    <mergeCell ref="A63:C63"/>
+    <mergeCell ref="D63:G63"/>
+    <mergeCell ref="H63:N63"/>
+    <mergeCell ref="O63:Q63"/>
+    <mergeCell ref="R63:S63"/>
+    <mergeCell ref="A67:C67"/>
+    <mergeCell ref="D67:G67"/>
+    <mergeCell ref="H67:N67"/>
+    <mergeCell ref="O67:Q67"/>
+    <mergeCell ref="R67:S67"/>
+    <mergeCell ref="A64:C64"/>
+    <mergeCell ref="D64:G64"/>
+    <mergeCell ref="H64:N64"/>
+    <mergeCell ref="O64:Q64"/>
+    <mergeCell ref="R64:S64"/>
+    <mergeCell ref="A65:C65"/>
+    <mergeCell ref="D65:G65"/>
+    <mergeCell ref="H65:N65"/>
+    <mergeCell ref="O65:Q65"/>
+    <mergeCell ref="R65:S65"/>
+    <mergeCell ref="A66:C66"/>
+    <mergeCell ref="D66:G66"/>
+    <mergeCell ref="H66:N66"/>
+    <mergeCell ref="O66:Q66"/>
+    <mergeCell ref="A60:C60"/>
+    <mergeCell ref="D60:G60"/>
+    <mergeCell ref="H60:N60"/>
+    <mergeCell ref="O60:Q60"/>
+    <mergeCell ref="R60:S60"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="D62:G62"/>
+    <mergeCell ref="H62:N62"/>
+    <mergeCell ref="O62:Q62"/>
+    <mergeCell ref="R62:S62"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="D56:G56"/>
+    <mergeCell ref="H56:N56"/>
+    <mergeCell ref="O56:Q56"/>
+    <mergeCell ref="R56:S56"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="D58:G58"/>
+    <mergeCell ref="H58:N58"/>
+    <mergeCell ref="O58:Q58"/>
+    <mergeCell ref="R58:S58"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="D47:G47"/>
+    <mergeCell ref="H47:N47"/>
+    <mergeCell ref="O47:Q47"/>
+    <mergeCell ref="R47:S47"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="D48:G48"/>
+    <mergeCell ref="H48:N48"/>
+    <mergeCell ref="O48:Q48"/>
+    <mergeCell ref="R48:S48"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="D44:G44"/>
+    <mergeCell ref="H44:N44"/>
+    <mergeCell ref="O44:Q44"/>
+    <mergeCell ref="R44:S44"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="D45:G45"/>
+    <mergeCell ref="H45:N45"/>
+    <mergeCell ref="O45:Q45"/>
+    <mergeCell ref="R45:S45"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="D38:G38"/>
+    <mergeCell ref="H38:N38"/>
+    <mergeCell ref="O38:Q38"/>
+    <mergeCell ref="R38:S38"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="D40:G40"/>
+    <mergeCell ref="H40:N40"/>
+    <mergeCell ref="O40:Q40"/>
+    <mergeCell ref="R40:S40"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="H27:N27"/>
+    <mergeCell ref="O27:Q27"/>
+    <mergeCell ref="R27:S27"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="D34:G34"/>
+    <mergeCell ref="H34:N34"/>
+    <mergeCell ref="O34:Q34"/>
+    <mergeCell ref="R34:S34"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="D29:G29"/>
+    <mergeCell ref="H29:N29"/>
+    <mergeCell ref="O29:Q29"/>
+    <mergeCell ref="R29:S29"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="D30:G30"/>
+    <mergeCell ref="H30:N30"/>
+    <mergeCell ref="O30:Q30"/>
+    <mergeCell ref="R30:S30"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="D31:G31"/>
+    <mergeCell ref="H31:N31"/>
+    <mergeCell ref="O31:Q31"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="D24:G24"/>
+    <mergeCell ref="H24:N24"/>
+    <mergeCell ref="O24:Q24"/>
+    <mergeCell ref="R24:S24"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="H1:N1"/>

</xml_diff>